<commit_message>
added new app notes and sub models
</commit_message>
<xml_diff>
--- a/src/main/resources/sum_app_notes.xlsx
+++ b/src/main/resources/sum_app_notes.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="696">
   <si>
     <t>delete</t>
   </si>
@@ -1726,17 +1726,424 @@
   <si>
     <t>For 1985-2005 Mazda B-series 1 tonne models.</t>
   </si>
+  <si>
+    <t>235/60R/16 Original Tire Size</t>
+  </si>
+  <si>
+    <t>Aspiration: Naturally Aspirated</t>
+  </si>
+  <si>
+    <t>Aspiration: Turbocharged</t>
+  </si>
+  <si>
+    <t>Constant Rate Spring</t>
+  </si>
+  <si>
+    <t>Engine VIN: 3</t>
+  </si>
+  <si>
+    <t>Engine VIN: P</t>
+  </si>
+  <si>
+    <t>Except GM Brake code JD3</t>
+  </si>
+  <si>
+    <t>Except GM Brake code JD5</t>
+  </si>
+  <si>
+    <t>Except Tahoe Package</t>
+  </si>
+  <si>
+    <t>Fuel Type: DIESEL</t>
+  </si>
+  <si>
+    <t>Fuel Type: GAS</t>
+  </si>
+  <si>
+    <t>GM Brake Code JB1</t>
+  </si>
+  <si>
+    <t>GM Brake Code JB3</t>
+  </si>
+  <si>
+    <t>GM Brake Code JB5</t>
+  </si>
+  <si>
+    <t>GM Brake Code JB6</t>
+  </si>
+  <si>
+    <t>GM Brake Code JB7</t>
+  </si>
+  <si>
+    <t>GM Brake code JD3</t>
+  </si>
+  <si>
+    <t>GM Brake code JD5</t>
+  </si>
+  <si>
+    <t>GM Brake Code JD7</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2</t>
+  </si>
+  <si>
+    <t>Number of Doors: 3</t>
+  </si>
+  <si>
+    <t>Number of Doors: 4</t>
+  </si>
+  <si>
+    <t>Problem Solver Design Features COATED FOR CORROSION RESISTANCE</t>
+  </si>
+  <si>
+    <t>Transmission Type: Transaxle</t>
+  </si>
+  <si>
+    <t>Transmission Type: Transmission</t>
+  </si>
+  <si>
+    <t>c/c/c/c</t>
+  </si>
+  <si>
+    <t>c/c/c/i</t>
+  </si>
+  <si>
+    <t>c/c/c/f</t>
+  </si>
+  <si>
+    <t>Aspiration: Naturally Aspirated, Number of Doors: 2</t>
+  </si>
+  <si>
+    <t>Aspiration: Naturally Aspirated, Number of Doors: 2, Transmission Type: Transaxle</t>
+  </si>
+  <si>
+    <t>Aspiration: Naturally Aspirated, Number of Doors: 2. Constant Rate Spring</t>
+  </si>
+  <si>
+    <t>Aspiration: Naturally Aspirated, Number of Doors: 4, Transmission Type: Transaxle</t>
+  </si>
+  <si>
+    <t>Aspiration: Naturally Aspirated. Constant Rate Spring</t>
+  </si>
+  <si>
+    <t>Aspiration: Naturally Aspirated. Superseded - Replaced by 6454B Neoprene Material</t>
+  </si>
+  <si>
+    <t>Aspiration: Turbocharged. Constant Rate Spring</t>
+  </si>
+  <si>
+    <t>Engine VIN: 3. Problem Solver Design Features COATED FOR CORROSION RESISTANCE</t>
+  </si>
+  <si>
+    <t>Engine VIN: P. Problem Solver Design Features COATED FOR CORROSION RESISTANCE</t>
+  </si>
+  <si>
+    <t>Fuel Type: DIESEL. Constant Rate Spring</t>
+  </si>
+  <si>
+    <t>Fuel Type: GAS. Constant Rate Spring</t>
+  </si>
+  <si>
+    <t>Fuel Type: GAS. Except 4.56 Gear Ratio</t>
+  </si>
+  <si>
+    <t>Fuel Type: GAS. GM Brake Code JB1</t>
+  </si>
+  <si>
+    <t>Fuel Type: GAS. GM Brake Code JB7</t>
+  </si>
+  <si>
+    <t>Fuel Type: GAS. GM Brake Code JD7</t>
+  </si>
+  <si>
+    <t>Fuel Type: GAS. Problem Solver Design Features COATED FOR CORROSION RESISTANCE</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2, Fuel Delivery Sub Type: 1BBL</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2, Fuel Delivery Sub Type: 1BBL, Transmission Type: Transaxle</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2, Fuel Delivery Sub Type: 1BBL. Constant Rate Spring</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2, Fuel Delivery Sub Type: 4BBL</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2, Fuel Delivery Sub Type: 4BBL. Constant Rate Spring</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2, Fuel Delivery Sub Type: MFI</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2, Fuel Delivery Sub Type: MFI, Transmission Type: Transaxle</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2, Fuel Type: DIESEL</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2, Fuel Type: DIESEL, Transmission Number of Speeds: 3, Transmission Type: Transmission</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2, Fuel Type: DIESEL, Transmission Type: Transmission</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2, Fuel Type: DIESEL, Transmission Type: Transmission. Constant Rate Spring</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2, Fuel Type: DIESEL, Transmission Type: Transmission. Except Gypsy Package</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2, Fuel Type: DIESEL. Constant Rate Spring</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2, Fuel Type: DIESEL. Except Gypsy Package</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2, Fuel Type: GAS</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2, Fuel Type: GAS. Constant Rate Spring</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2, Fuel Type: GAS. Except Gypsy Package</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2, Transmission Number of Speeds: 3, Transmission Type: Transmission</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2, Transmission Number of Speeds: 3, Transmission Type: Transmission. Constant Rate Spring</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2, Transmission Number of Speeds: 3, Transmission Type: Transmission. Except Gypsy Package</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2, Transmission Number of Speeds: 3, Transmission Type: Transmission. Except Tahoe Package</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2, Transmission Number of Speeds: 4, Transmission Type: Transaxle</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2, Transmission Type: Transaxle</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2, Transmission Type: Transaxle. Constant Rate Spring</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2, Transmission Type: Transmission</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2, Transmission Type: Transmission. Constant Rate Spring</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2, Transmission Type: Transmission. Except Gypsy Package</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2, Transmission Type: Transmission. Except Tahoe Package</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2. 215/70R/16 Original Tire Size</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2. Constant Rate Spring</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2. Except EL Package</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2. Except Gypsy Package</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2. Except Tahoe Package</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2. GM Brake Code JB6</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2. GM Brake Code JB7</t>
+  </si>
+  <si>
+    <t>Number of Doors: 2. GM Brake Code JD6</t>
+  </si>
+  <si>
+    <t>Number of Doors: 3. Constant Rate Spring</t>
+  </si>
+  <si>
+    <t>Number of Doors: 4, Fuel Delivery Sub Type: 1BBL, Transmission Type: Transaxle</t>
+  </si>
+  <si>
+    <t>Number of Doors: 4, Fuel Delivery Sub Type: MFI</t>
+  </si>
+  <si>
+    <t>Number of Doors: 4, Fuel Delivery Sub Type: MFI, Transmission Type: Transaxle</t>
+  </si>
+  <si>
+    <t>Number of Doors: 4, Fuel Type: DIESEL</t>
+  </si>
+  <si>
+    <t>Number of Doors: 4, Fuel Type: DIESEL, Transmission Type: Transmission</t>
+  </si>
+  <si>
+    <t>Number of Doors: 4, Fuel Type: DIESEL, Transmission Type: Transmission. Constant Rate Spring</t>
+  </si>
+  <si>
+    <t>Number of Doors: 4, Fuel Type: DIESEL. Constant Rate Spring</t>
+  </si>
+  <si>
+    <t>Number of Doors: 4, Fuel Type: GAS</t>
+  </si>
+  <si>
+    <t>Number of Doors: 4, Fuel Type: GAS. Constant Rate Spring</t>
+  </si>
+  <si>
+    <t>Number of Doors: 4, Transmission Number of Speeds: 3, Transmission Type: Transmission</t>
+  </si>
+  <si>
+    <t>Number of Doors: 4, Transmission Number of Speeds: 3, Transmission Type: Transmission. Constant Rate Spring</t>
+  </si>
+  <si>
+    <t>Number of Doors: 4, Transmission Number of Speeds: 4, Transmission Type: Transaxle</t>
+  </si>
+  <si>
+    <t>Number of Doors: 4, Transmission Number of Speeds: 4, Transmission Type: Transmission</t>
+  </si>
+  <si>
+    <t>Number of Doors: 4, Transmission Number of Speeds: 4, Transmission Type: Transmission. Constant Rate Spring</t>
+  </si>
+  <si>
+    <t>Number of Doors: 4, Transmission Type: Transaxle</t>
+  </si>
+  <si>
+    <t>Number of Doors: 4, Transmission Type: Transaxle. Constant Rate Spring</t>
+  </si>
+  <si>
+    <t>Number of Doors: 4, Transmission Type: Transmission</t>
+  </si>
+  <si>
+    <t>Number of Doors: 4, Transmission Type: Transmission. Constant Rate Spring</t>
+  </si>
+  <si>
+    <t>Number of Doors: 4. 235/60R/16 Original Tire Size</t>
+  </si>
+  <si>
+    <t>Number of Doors: 4. Constant Rate Spring</t>
+  </si>
+  <si>
+    <t>Transmission Number of Speeds: 3, Transmission Type: Transmission</t>
+  </si>
+  <si>
+    <t>Transmission Number of Speeds: 3, Transmission Type: Transmission. Constant Rate Spring</t>
+  </si>
+  <si>
+    <t>Transmission Number of Speeds: 3, Transmission Type: Transmission. Except Tahoe Package</t>
+  </si>
+  <si>
+    <t>Transmission Number of Speeds: 4, Transmission Type: Transmission</t>
+  </si>
+  <si>
+    <t>Transmission Number of Speeds: 4, Transmission Type: Transmission. Constant Rate Spring</t>
+  </si>
+  <si>
+    <t>Transmission Type: Transaxle. Constant Rate Spring</t>
+  </si>
+  <si>
+    <t>Transmission Type: Transmission. Constant Rate Spring</t>
+  </si>
+  <si>
+    <t>Transmission Type: Transmission. Except Tahoe Package</t>
+  </si>
+  <si>
+    <t>Wheel Base US: 108.0, Number of Doors: 2</t>
+  </si>
+  <si>
+    <t>Wheel Base US: 108.0, Number of Doors: 2, Fuel Type: GAS</t>
+  </si>
+  <si>
+    <t>Wheel Base US: 108.0, Transmission Type: Transmission</t>
+  </si>
+  <si>
+    <t>Wheel Base US: 112.0, Number of Doors: 2</t>
+  </si>
+  <si>
+    <t>Wheel Base US: 112.0, Number of Doors: 2, Transmission Type: Transmission</t>
+  </si>
+  <si>
+    <t>Wheel Base US: 112.0, Number of Doors: 2, Transmission Type: Transmission. Constant Rate Spring</t>
+  </si>
+  <si>
+    <t>Wheel Base US: 112.0, Number of Doors: 2. Constant Rate Spring</t>
+  </si>
+  <si>
+    <t>Wheel Base US: 114.0, Number of Doors: 2, Fuel Type: GAS, Transmission Type: Transmission</t>
+  </si>
+  <si>
+    <t>Wheel Base US: 114.0, Transmission Type: Transmission</t>
+  </si>
+  <si>
+    <t>Wheel Base US: 135.5, Number of Doors: 2</t>
+  </si>
+  <si>
+    <t>Wheel Base US: 135.5, Number of Doors: 2. Constant Rate Spring</t>
+  </si>
+  <si>
+    <t>Wheel Base US: 159.5, Number of Doors: 2</t>
+  </si>
+  <si>
+    <t>c/с</t>
+  </si>
+  <si>
+    <t>c/с/с</t>
+  </si>
+  <si>
+    <t>c/i</t>
+  </si>
+  <si>
+    <t>c/с/i</t>
+  </si>
+  <si>
+    <t>c/с/c</t>
+  </si>
+  <si>
+    <t>c/с/c/i</t>
+  </si>
+  <si>
+    <t>c/с/c/f</t>
+  </si>
+  <si>
+    <t>c/с/f</t>
+  </si>
+  <si>
+    <t>c/c/c</t>
+  </si>
+  <si>
+    <t>c/c</t>
+  </si>
+  <si>
+    <t>c/c/i</t>
+  </si>
+  <si>
+    <t>c/c/f</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="68" x14ac:knownFonts="1">
+  <fonts count="69" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2326,18 +2733,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="67" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2361,7 +2771,7 @@
     <xf numFmtId="0" fontId="57" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2373,10 +2783,10 @@
     <xf numFmtId="0" fontId="54" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2529,7 +2939,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2812,10 +3225,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B580"/>
+  <dimension ref="A1:B699"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A567" workbookViewId="0">
-      <selection activeCell="B587" sqref="B587"/>
+    <sheetView tabSelected="1" topLeftCell="A566" workbookViewId="0">
+      <selection activeCell="A699" sqref="A699"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7455,13 +7868,960 @@
         <v>561</v>
       </c>
     </row>
-    <row r="580" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="580" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A580" s="68" t="s">
         <v>4</v>
       </c>
       <c r="B580" t="s">
         <v>562</v>
       </c>
+    </row>
+    <row r="581" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A581" s="70" t="s">
+        <v>2</v>
+      </c>
+      <c r="B581" s="70" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="582" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A582" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="B582" s="69" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="583" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A583" s="70" t="s">
+        <v>684</v>
+      </c>
+      <c r="B583" s="69" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="584" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A584" s="70" t="s">
+        <v>685</v>
+      </c>
+      <c r="B584" s="69" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="585" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A585" s="70" t="s">
+        <v>687</v>
+      </c>
+      <c r="B585" s="69" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="586" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A586" s="70" t="s">
+        <v>685</v>
+      </c>
+      <c r="B586" s="69" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="587" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A587" s="70" t="s">
+        <v>686</v>
+      </c>
+      <c r="B587" s="69" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="588" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A588" s="70" t="s">
+        <v>686</v>
+      </c>
+      <c r="B588" s="69" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="589" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A589" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="B589" s="70" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="590" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A590" s="70" t="s">
+        <v>686</v>
+      </c>
+      <c r="B590" s="69" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="591" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A591" s="70" t="s">
+        <v>6</v>
+      </c>
+      <c r="B591" s="70" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="592" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A592" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="B592" s="70" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="593" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A593" s="70" t="s">
+        <v>686</v>
+      </c>
+      <c r="B593" s="69" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="594" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A594" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="B594" s="70" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="595" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A595" s="70" t="s">
+        <v>686</v>
+      </c>
+      <c r="B595" s="69" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="596" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A596" s="70" t="s">
+        <v>2</v>
+      </c>
+      <c r="B596" s="70" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="597" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A597" s="70" t="s">
+        <v>2</v>
+      </c>
+      <c r="B597" s="70" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="598" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A598" s="70" t="s">
+        <v>2</v>
+      </c>
+      <c r="B598" s="70" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="599" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A599" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="B599" s="70" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="600" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A600" s="70" t="s">
+        <v>686</v>
+      </c>
+      <c r="B600" s="69" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="601" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A601" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="B601" s="70" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="602" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A602" s="70" t="s">
+        <v>686</v>
+      </c>
+      <c r="B602" s="69" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="603" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A603" s="70" t="s">
+        <v>58</v>
+      </c>
+      <c r="B603" s="69" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="604" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A604" s="70" t="s">
+        <v>58</v>
+      </c>
+      <c r="B604" s="69" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="605" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A605" s="70" t="s">
+        <v>58</v>
+      </c>
+      <c r="B605" s="69" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="606" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A606" s="70" t="s">
+        <v>58</v>
+      </c>
+      <c r="B606" s="69" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="607" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A607" s="70" t="s">
+        <v>686</v>
+      </c>
+      <c r="B607" s="69" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="608" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A608" s="70" t="s">
+        <v>2</v>
+      </c>
+      <c r="B608" s="70" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="609" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A609" s="70" t="s">
+        <v>2</v>
+      </c>
+      <c r="B609" s="70" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="610" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A610" s="70" t="s">
+        <v>2</v>
+      </c>
+      <c r="B610" s="70" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="611" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A611" s="70" t="s">
+        <v>2</v>
+      </c>
+      <c r="B611" s="70" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="612" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A612" s="70" t="s">
+        <v>2</v>
+      </c>
+      <c r="B612" s="70" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="613" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A613" s="70" t="s">
+        <v>2</v>
+      </c>
+      <c r="B613" s="70" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="614" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A614" s="70" t="s">
+        <v>2</v>
+      </c>
+      <c r="B614" s="70" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="615" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A615" s="70" t="s">
+        <v>2</v>
+      </c>
+      <c r="B615" s="70" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="616" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A616" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="B616" s="70" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="617" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A617" s="70" t="s">
+        <v>684</v>
+      </c>
+      <c r="B617" s="69" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="618" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A618" s="70" t="s">
+        <v>685</v>
+      </c>
+      <c r="B618" s="69" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="619" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A619" s="70" t="s">
+        <v>687</v>
+      </c>
+      <c r="B619" s="69" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="620" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A620" s="70" t="s">
+        <v>684</v>
+      </c>
+      <c r="B620" s="69" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="621" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A621" s="70" t="s">
+        <v>687</v>
+      </c>
+      <c r="B621" s="69" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="622" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A622" s="70" t="s">
+        <v>684</v>
+      </c>
+      <c r="B622" s="69" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="623" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A623" s="70" t="s">
+        <v>688</v>
+      </c>
+      <c r="B623" s="69" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="624" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A624" s="70" t="s">
+        <v>684</v>
+      </c>
+      <c r="B624" s="69" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="625" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A625" s="70" t="s">
+        <v>588</v>
+      </c>
+      <c r="B625" s="69" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="626" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A626" s="70" t="s">
+        <v>688</v>
+      </c>
+      <c r="B626" s="69" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="627" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A627" s="70" t="s">
+        <v>689</v>
+      </c>
+      <c r="B627" s="69" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="628" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A628" s="70" t="s">
+        <v>690</v>
+      </c>
+      <c r="B628" s="69" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="629" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A629" s="70" t="s">
+        <v>687</v>
+      </c>
+      <c r="B629" s="69" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="630" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A630" s="70" t="s">
+        <v>691</v>
+      </c>
+      <c r="B630" s="69" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="631" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A631" s="70" t="s">
+        <v>684</v>
+      </c>
+      <c r="B631" s="69" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="632" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A632" s="70" t="s">
+        <v>687</v>
+      </c>
+      <c r="B632" s="69" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="633" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A633" s="70" t="s">
+        <v>691</v>
+      </c>
+      <c r="B633" s="69" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="634" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A634" s="70" t="s">
+        <v>692</v>
+      </c>
+      <c r="B634" s="69" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="635" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A635" s="70" t="s">
+        <v>589</v>
+      </c>
+      <c r="B635" s="69" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="636" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A636" s="70" t="s">
+        <v>590</v>
+      </c>
+      <c r="B636" s="69" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="637" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A637" s="70" t="s">
+        <v>590</v>
+      </c>
+      <c r="B637" s="69" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="638" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A638" s="70" t="s">
+        <v>692</v>
+      </c>
+      <c r="B638" s="69" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="639" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A639" s="70" t="s">
+        <v>693</v>
+      </c>
+      <c r="B639" s="69" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="640" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A640" s="70" t="s">
+        <v>694</v>
+      </c>
+      <c r="B640" s="69" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="641" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A641" s="70" t="s">
+        <v>693</v>
+      </c>
+      <c r="B641" s="69" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="642" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A642" s="70" t="s">
+        <v>694</v>
+      </c>
+      <c r="B642" s="69" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="643" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A643" s="70" t="s">
+        <v>695</v>
+      </c>
+      <c r="B643" s="69" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="644" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A644" s="70" t="s">
+        <v>695</v>
+      </c>
+      <c r="B644" s="69" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="645" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A645" s="70" t="s">
+        <v>58</v>
+      </c>
+      <c r="B645" s="69" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="646" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A646" s="70" t="s">
+        <v>686</v>
+      </c>
+      <c r="B646" s="69" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="647" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A647" s="70" t="s">
+        <v>58</v>
+      </c>
+      <c r="B647" s="69" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="648" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A648" s="70" t="s">
+        <v>58</v>
+      </c>
+      <c r="B648" s="69" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="649" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A649" s="70" t="s">
+        <v>58</v>
+      </c>
+      <c r="B649" s="69" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="650" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A650" s="70" t="s">
+        <v>58</v>
+      </c>
+      <c r="B650" s="69" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="651" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A651" s="70" t="s">
+        <v>58</v>
+      </c>
+      <c r="B651" s="69" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="652" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A652" s="70" t="s">
+        <v>58</v>
+      </c>
+      <c r="B652" s="69" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="653" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A653" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="B653" s="70" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="654" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A654" s="70" t="s">
+        <v>686</v>
+      </c>
+      <c r="B654" s="69" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="655" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A655" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="B655" s="70" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="656" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A656" s="70" t="s">
+        <v>692</v>
+      </c>
+      <c r="B656" s="69" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="657" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A657" s="70" t="s">
+        <v>693</v>
+      </c>
+      <c r="B657" s="69" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="658" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A658" s="70" t="s">
+        <v>692</v>
+      </c>
+      <c r="B658" s="69" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="659" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A659" s="70" t="s">
+        <v>693</v>
+      </c>
+      <c r="B659" s="69" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="660" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A660" s="70" t="s">
+        <v>692</v>
+      </c>
+      <c r="B660" s="69" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="661" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A661" s="70" t="s">
+        <v>589</v>
+      </c>
+      <c r="B661" s="69" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="662" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A662" s="70" t="s">
+        <v>694</v>
+      </c>
+      <c r="B662" s="69" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="663" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A663" s="70" t="s">
+        <v>693</v>
+      </c>
+      <c r="B663" s="69" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="664" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A664" s="70" t="s">
+        <v>694</v>
+      </c>
+      <c r="B664" s="69" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="665" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A665" s="70" t="s">
+        <v>692</v>
+      </c>
+      <c r="B665" s="69" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="666" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A666" s="70" t="s">
+        <v>589</v>
+      </c>
+      <c r="B666" s="69" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="667" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A667" s="70" t="s">
+        <v>692</v>
+      </c>
+      <c r="B667" s="69" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="668" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A668" s="70" t="s">
+        <v>692</v>
+      </c>
+      <c r="B668" s="69" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="669" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A669" s="70" t="s">
+        <v>589</v>
+      </c>
+      <c r="B669" s="69" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="670" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A670" s="70" t="s">
+        <v>693</v>
+      </c>
+      <c r="B670" s="69" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="671" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A671" s="70" t="s">
+        <v>694</v>
+      </c>
+      <c r="B671" s="69" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="672" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A672" s="70" t="s">
+        <v>693</v>
+      </c>
+      <c r="B672" s="69" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="673" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A673" s="70" t="s">
+        <v>694</v>
+      </c>
+      <c r="B673" s="69" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="674" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A674" s="70" t="s">
+        <v>58</v>
+      </c>
+      <c r="B674" s="69" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="675" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A675" s="70" t="s">
+        <v>686</v>
+      </c>
+      <c r="B675" s="69" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="676" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A676" s="70" t="s">
+        <v>6</v>
+      </c>
+      <c r="B676" s="69" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="677" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A677" s="70" t="s">
+        <v>693</v>
+      </c>
+      <c r="B677" s="69" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="678" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A678" s="70" t="s">
+        <v>694</v>
+      </c>
+      <c r="B678" s="69" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="679" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A679" s="70" t="s">
+        <v>695</v>
+      </c>
+      <c r="B679" s="69" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="680" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A680" s="70" t="s">
+        <v>693</v>
+      </c>
+      <c r="B680" s="69" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="681" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A681" s="70" t="s">
+        <v>694</v>
+      </c>
+      <c r="B681" s="69" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="682" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A682" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="B682" s="70" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="683" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A683" s="70" t="s">
+        <v>686</v>
+      </c>
+      <c r="B683" s="69" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="684" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A684" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="B684" s="69" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="685" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A685" s="70" t="s">
+        <v>686</v>
+      </c>
+      <c r="B685" s="69" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="686" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A686" s="70" t="s">
+        <v>58</v>
+      </c>
+      <c r="B686" s="69" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="687" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A687" s="70" t="s">
+        <v>693</v>
+      </c>
+      <c r="B687" s="69" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="688" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A688" s="70" t="s">
+        <v>692</v>
+      </c>
+      <c r="B688" s="69" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="689" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A689" s="70" t="s">
+        <v>693</v>
+      </c>
+      <c r="B689" s="69" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="690" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A690" s="70" t="s">
+        <v>693</v>
+      </c>
+      <c r="B690" s="69" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="691" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A691" s="70" t="s">
+        <v>692</v>
+      </c>
+      <c r="B691" s="69" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="692" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A692" s="70" t="s">
+        <v>589</v>
+      </c>
+      <c r="B692" s="69" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="693" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A693" s="70" t="s">
+        <v>694</v>
+      </c>
+      <c r="B693" s="69" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="694" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A694" s="70" t="s">
+        <v>588</v>
+      </c>
+      <c r="B694" s="69" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="695" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A695" s="70" t="s">
+        <v>693</v>
+      </c>
+      <c r="B695" s="69" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="696" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A696" s="70" t="s">
+        <v>693</v>
+      </c>
+      <c r="B696" s="69" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="697" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A697" s="70" t="s">
+        <v>694</v>
+      </c>
+      <c r="B697" s="69" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="698" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A698" s="70" t="s">
+        <v>693</v>
+      </c>
+      <c r="B698" s="69" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="699" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A699" s="70"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:B561"/>

</xml_diff>

<commit_message>
added complex app note split
</commit_message>
<xml_diff>
--- a/src/main/resources/sum_app_notes.xlsx
+++ b/src/main/resources/sum_app_notes.xlsx
@@ -3225,10 +3225,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B699"/>
+  <dimension ref="A1:B698"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A566" workbookViewId="0">
-      <selection activeCell="A699" sqref="A699"/>
+    <sheetView tabSelected="1" topLeftCell="A679" workbookViewId="0">
+      <selection activeCell="J697" sqref="J697"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8820,9 +8820,6 @@
         <v>683</v>
       </c>
     </row>
-    <row r="699" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A699" s="70"/>
-    </row>
   </sheetData>
   <autoFilter ref="A1:B561"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
minor summit import fixes
</commit_message>
<xml_diff>
--- a/src/main/resources/sum_app_notes.xlsx
+++ b/src/main/resources/sum_app_notes.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249A4658-BBFD-4124-BBDD-A4270AA8F515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7352E77-A2C2-4643-B54A-DDCFE2FEBC3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2675,60 +2675,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2876,69 +2828,66 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -3221,8 +3170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B865"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A843" workbookViewId="0">
-      <selection activeCell="B862" sqref="B862:B865"/>
+    <sheetView tabSelected="1" topLeftCell="A802" workbookViewId="0">
+      <selection activeCell="A814" sqref="A814:B865"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9736,266 +9685,266 @@
       </c>
     </row>
     <row r="814" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A814" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B814" s="19" t="s">
+      <c r="A814" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B814" s="20" t="s">
         <v>813</v>
       </c>
     </row>
     <row r="815" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A815" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B815" s="19" t="s">
+      <c r="A815" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B815" s="20" t="s">
         <v>814</v>
       </c>
     </row>
     <row r="816" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A816" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B816" s="19" t="s">
+      <c r="A816" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B816" s="20" t="s">
         <v>815</v>
       </c>
     </row>
     <row r="817" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A817" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B817" s="19" t="s">
+      <c r="A817" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B817" s="20" t="s">
         <v>816</v>
       </c>
     </row>
     <row r="818" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A818" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B818" s="19" t="s">
+      <c r="A818" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B818" s="20" t="s">
         <v>817</v>
       </c>
     </row>
     <row r="819" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A819" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B819" s="19" t="s">
+      <c r="A819" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B819" s="20" t="s">
         <v>818</v>
       </c>
     </row>
     <row r="820" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A820" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B820" s="20" t="s">
+      <c r="A820" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B820" s="21" t="s">
         <v>819</v>
       </c>
     </row>
     <row r="821" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A821" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B821" s="19" t="s">
+      <c r="A821" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B821" s="20" t="s">
         <v>820</v>
       </c>
     </row>
     <row r="822" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A822" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B822" s="19" t="s">
+      <c r="A822" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B822" s="20" t="s">
         <v>821</v>
       </c>
     </row>
     <row r="823" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A823" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B823" s="19" t="s">
+      <c r="A823" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B823" s="20" t="s">
         <v>822</v>
       </c>
     </row>
     <row r="824" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A824" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B824" s="19" t="s">
+      <c r="A824" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B824" s="20" t="s">
         <v>823</v>
       </c>
     </row>
     <row r="825" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A825" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B825" s="19" t="s">
+      <c r="A825" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B825" s="20" t="s">
         <v>824</v>
       </c>
     </row>
     <row r="826" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A826" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B826" s="19" t="s">
+      <c r="A826" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B826" s="20" t="s">
         <v>825</v>
       </c>
     </row>
     <row r="827" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A827" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B827" s="19" t="s">
+      <c r="A827" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B827" s="20" t="s">
         <v>826</v>
       </c>
     </row>
     <row r="828" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A828" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B828" s="19" t="s">
+      <c r="A828" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B828" s="20" t="s">
         <v>827</v>
       </c>
     </row>
     <row r="829" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A829" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B829" s="19" t="s">
+      <c r="A829" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B829" s="20" t="s">
         <v>828</v>
       </c>
     </row>
     <row r="830" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A830" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B830" s="19" t="s">
+      <c r="A830" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B830" s="20" t="s">
         <v>829</v>
       </c>
     </row>
     <row r="831" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A831" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B831" s="20" t="s">
+      <c r="A831" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B831" s="21" t="s">
         <v>830</v>
       </c>
     </row>
     <row r="832" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A832" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B832" s="20" t="s">
+      <c r="A832" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B832" s="21" t="s">
         <v>831</v>
       </c>
     </row>
     <row r="833" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A833" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B833" s="19" t="s">
+      <c r="A833" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B833" s="20" t="s">
         <v>832</v>
       </c>
     </row>
     <row r="834" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A834" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B834" s="19" t="s">
+      <c r="A834" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B834" s="20" t="s">
         <v>833</v>
       </c>
     </row>
     <row r="835" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A835" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B835" s="19" t="s">
+      <c r="A835" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B835" s="20" t="s">
         <v>834</v>
       </c>
     </row>
     <row r="836" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A836" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B836" s="19" t="s">
+      <c r="A836" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B836" s="20" t="s">
         <v>835</v>
       </c>
     </row>
     <row r="837" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A837" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B837" s="19" t="s">
+      <c r="A837" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B837" s="20" t="s">
         <v>836</v>
       </c>
     </row>
     <row r="838" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A838" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B838" s="19" t="s">
+      <c r="A838" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B838" s="20" t="s">
         <v>837</v>
       </c>
     </row>
     <row r="839" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A839" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B839" s="19" t="s">
+      <c r="A839" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B839" s="20" t="s">
         <v>838</v>
       </c>
     </row>
     <row r="840" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A840" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B840" s="19" t="s">
+      <c r="A840" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B840" s="20" t="s">
         <v>839</v>
       </c>
     </row>
     <row r="841" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A841" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B841" s="19" t="s">
+      <c r="A841" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B841" s="20" t="s">
         <v>840</v>
       </c>
     </row>
     <row r="842" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A842" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B842" s="19" t="s">
+      <c r="A842" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B842" s="20" t="s">
         <v>841</v>
       </c>
     </row>
     <row r="843" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A843" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B843" s="19" t="s">
+      <c r="A843" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B843" s="20" t="s">
         <v>842</v>
       </c>
     </row>
     <row r="844" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A844" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B844" s="19" t="s">
+      <c r="A844" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B844" s="20" t="s">
         <v>843</v>
       </c>
     </row>
     <row r="845" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A845" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B845" s="19" t="s">
+      <c r="A845" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B845" s="20" t="s">
         <v>844</v>
       </c>
     </row>
     <row r="846" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A846" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="B846" s="19" t="s">
+      <c r="A846" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B846" s="20" t="s">
         <v>845</v>
       </c>
     </row>
@@ -10003,7 +9952,7 @@
       <c r="A847" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B847" s="19" t="s">
+      <c r="B847" s="20" t="s">
         <v>846</v>
       </c>
     </row>
@@ -10011,143 +9960,143 @@
       <c r="A848" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B848" s="19" t="s">
+      <c r="B848" s="20" t="s">
         <v>847</v>
       </c>
     </row>
     <row r="849" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A849" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B849" s="19" t="s">
+      <c r="A849" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B849" s="20" t="s">
         <v>848</v>
       </c>
     </row>
     <row r="850" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A850" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B850" s="19" t="s">
+      <c r="A850" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B850" s="20" t="s">
         <v>849</v>
       </c>
     </row>
     <row r="851" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A851" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B851" s="11" t="s">
+      <c r="A851" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B851" t="s">
         <v>850</v>
       </c>
     </row>
     <row r="852" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A852" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B852" s="11" t="s">
+      <c r="A852" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B852" t="s">
         <v>851</v>
       </c>
     </row>
     <row r="853" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A853" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B853" s="11" t="s">
+      <c r="A853" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B853" t="s">
         <v>852</v>
       </c>
     </row>
     <row r="854" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A854" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B854" s="11" t="s">
+      <c r="A854" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B854" t="s">
         <v>853</v>
       </c>
     </row>
     <row r="855" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A855" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B855" s="11" t="s">
+      <c r="A855" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B855" t="s">
         <v>854</v>
       </c>
     </row>
     <row r="856" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A856" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B856" s="11" t="s">
+      <c r="A856" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B856" t="s">
         <v>855</v>
       </c>
     </row>
     <row r="857" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A857" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B857" s="11" t="s">
+      <c r="A857" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B857" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="858" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A858" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B858" s="11" t="s">
+      <c r="A858" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B858" t="s">
         <v>857</v>
       </c>
     </row>
     <row r="859" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A859" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B859" s="11" t="s">
+      <c r="A859" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B859" t="s">
         <v>858</v>
       </c>
     </row>
     <row r="860" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A860" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B860" s="11" t="s">
+      <c r="A860" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B860" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="861" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A861" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B861" s="11" t="s">
+      <c r="A861" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B861" t="s">
         <v>859</v>
       </c>
     </row>
     <row r="862" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A862" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="B862" s="11" t="s">
+      <c r="A862" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B862" t="s">
         <v>860</v>
       </c>
     </row>
     <row r="863" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A863" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="B863" s="11" t="s">
+      <c r="A863" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B863" t="s">
         <v>861</v>
       </c>
     </row>
     <row r="864" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A864" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="B864" s="11" t="s">
+      <c r="A864" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B864" t="s">
         <v>862</v>
       </c>
     </row>
     <row r="865" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A865" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="B865" s="11" t="s">
+      <c r="A865" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B865" t="s">
         <v>863</v>
       </c>
     </row>

</xml_diff>

<commit_message>
implemented summit app notes check by brand
</commit_message>
<xml_diff>
--- a/src/main/resources/sum_app_notes.xlsx
+++ b/src/main/resources/sum_app_notes.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB870F0-4537-4EF7-95C6-2ECDA736CDC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA365E5-949D-4CEF-9860-6CB04E10095A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4036" uniqueCount="1991">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4078" uniqueCount="2010">
   <si>
     <t>[Available While Supplies Last]</t>
   </si>
@@ -6080,17 +6080,82 @@
   <si>
     <t>Conventional Cab w/19000, 21000, 23000 lb Taperleaf Springs (EXC Low Profile Vehicle) OEM #'S 15123676, 15174898, 15588554, 15887728, 19152843, 22064230, 88982682, 22064233, 88982684</t>
   </si>
+  <si>
+    <t>COLOR: ALUMINUM</t>
+  </si>
+  <si>
+    <t>RESERVOIR: REMOTE</t>
+  </si>
+  <si>
+    <t>SERIES: PERFORMANCE</t>
+  </si>
+  <si>
+    <t>SIZE: 2.0</t>
+  </si>
+  <si>
+    <t>Manufacturer Body Code: XJ</t>
+  </si>
+  <si>
+    <t>Manufacturer Body Code: MJ</t>
+  </si>
+  <si>
+    <t>Manufacturer Body Code: ZJ</t>
+  </si>
+  <si>
+    <t>Manufacturer Body Code: WJ</t>
+  </si>
+  <si>
+    <t>Manufacturer Body Code: JT</t>
+  </si>
+  <si>
+    <t>Manufacturer Body Code: JL</t>
+  </si>
+  <si>
+    <t>Manufacturer Body Code: JK</t>
+  </si>
+  <si>
+    <t>Body Type: Extended Cab Pickup</t>
+  </si>
+  <si>
+    <t>Body Type: Standard Cab Pickup</t>
+  </si>
+  <si>
+    <t>Body Type: Cab &amp; Chassis</t>
+  </si>
+  <si>
+    <t>Fits cab &amp; chassis models.</t>
+  </si>
+  <si>
+    <t>Body Type: Cab &amp; Chassis - Conventional</t>
+  </si>
+  <si>
+    <t>Body Type: Cab &amp; Chassis - Crew Cab</t>
+  </si>
+  <si>
+    <t>Body Type: Cab &amp; Chassis - Extended Cab</t>
+  </si>
+  <si>
+    <t>Lift: 0-2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -6448,271 +6513,272 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="22" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -6993,10 +7059,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2018"/>
+  <dimension ref="A1:B2039"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1925" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B1939" sqref="B1939"/>
+    <sheetView tabSelected="1" topLeftCell="A2024" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2042" sqref="B2042"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23149,6 +23215,174 @@
         <v>1989</v>
       </c>
     </row>
+    <row r="2019" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2019" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2019" s="19" t="s">
+        <v>1991</v>
+      </c>
+    </row>
+    <row r="2020" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2020" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2020" s="19" t="s">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="2021" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2021" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2021" s="19" t="s">
+        <v>1993</v>
+      </c>
+    </row>
+    <row r="2022" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2022" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2022" s="19" t="s">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="2023" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2023" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2023" s="19" t="s">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="2024" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2024" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2024" s="19" t="s">
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="2025" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2025" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2025" s="19" t="s">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="2026" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2026" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2026" s="19" t="s">
+        <v>1998</v>
+      </c>
+    </row>
+    <row r="2027" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2027" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2027" s="19" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="2028" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2028" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2028" s="19" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="2029" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2029" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2029" s="19" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="2030" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2030" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2030" s="19" t="s">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="2031" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2031" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2031" s="19" t="s">
+        <v>1433</v>
+      </c>
+    </row>
+    <row r="2032" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2032" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2032" s="19" t="s">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="2033" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2033" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2033" s="19" t="s">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="2034" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2034" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2034" s="19" t="s">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="2035" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2035" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2035" s="19" t="s">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="2036" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2036" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2036" s="19" t="s">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="2037" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2037" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2037" s="19" t="s">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="2038" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2038" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2038" s="19" t="s">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="2039" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2039" s="98" t="s">
+        <v>283</v>
+      </c>
+      <c r="B2039" s="19" t="s">
+        <v>2009</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>